<commit_message>
as good as it gets
</commit_message>
<xml_diff>
--- a/2025_election_predictions.xlsx
+++ b/2025_election_predictions.xlsx
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4889610636550767</v>
+        <v>0.4986999471354288</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5110389363449233</v>
+        <v>0.5013000528645712</v>
       </c>
     </row>
     <row r="5">
@@ -513,7 +513,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -527,7 +527,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -545,10 +545,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5180940068063941</v>
+        <v>0.5213918732611434</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4819059931936058</v>
+        <v>0.4786081267388564</v>
       </c>
     </row>
     <row r="8">
@@ -559,7 +559,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -587,7 +587,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -605,10 +605,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5637822502464083</v>
+        <v>0.5692839823501323</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4362177497535918</v>
+        <v>0.4307160176498677</v>
       </c>
     </row>
     <row r="12">
@@ -675,7 +675,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5282952703833925</v>
+        <v>0.5310794522270156</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4717047296166075</v>
+        <v>0.4689205477729845</v>
       </c>
     </row>
     <row r="19">
@@ -767,10 +767,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5426656043626547</v>
+        <v>0.5447250124667524</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4573343956373453</v>
+        <v>0.4552749875332476</v>
       </c>
     </row>
     <row r="23">
@@ -785,10 +785,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5451830479927785</v>
+        <v>0.537870978919868</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4548169520072216</v>
+        <v>0.4621290210801319</v>
       </c>
     </row>
     <row r="24">
@@ -799,7 +799,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -813,7 +813,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -827,7 +827,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -859,10 +859,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.486202778353176</v>
+        <v>0.491102133507783</v>
       </c>
       <c r="D28" t="n">
-        <v>0.513797221646824</v>
+        <v>0.5088978664922169</v>
       </c>
     </row>
     <row r="29">
@@ -901,7 +901,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -933,10 +933,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.4765708282371158</v>
+        <v>0.4718533505002138</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5234291717628842</v>
+        <v>0.5281466494997862</v>
       </c>
     </row>
     <row r="34">
@@ -947,7 +947,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -975,7 +975,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -993,10 +993,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.5339574664628861</v>
+        <v>0.5411531160569628</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4660425335371139</v>
+        <v>0.4588468839430372</v>
       </c>
     </row>
     <row r="38">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.4648773638239581</v>
+        <v>0.4605997705688807</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5351226361760419</v>
+        <v>0.5394002294311193</v>
       </c>
     </row>
     <row r="40">
@@ -1057,10 +1057,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.5816301228285838</v>
+        <v>0.5817175396086411</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4183698771714162</v>
+        <v>0.4182824603913588</v>
       </c>
     </row>
     <row r="42">
@@ -1075,10 +1075,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.520224448717577</v>
+        <v>0.5281978769981704</v>
       </c>
       <c r="D42" t="n">
-        <v>0.4797755512824229</v>
+        <v>0.4718021230018296</v>
       </c>
     </row>
   </sheetData>
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4504170482467472</v>
+        <v>0.4523889073091529</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5495829517532527</v>
+        <v>0.5476110926908471</v>
       </c>
     </row>
     <row r="5">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1208,10 +1208,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.485670021164641</v>
+        <v>0.4860478629936003</v>
       </c>
       <c r="D7" t="n">
-        <v>0.514329978835359</v>
+        <v>0.5139521370063997</v>
       </c>
     </row>
     <row r="8">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1268,10 +1268,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5390517578376165</v>
+        <v>0.5400631779254161</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4609482421623834</v>
+        <v>0.4599368220745839</v>
       </c>
     </row>
     <row r="12">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.4977870438157466</v>
+        <v>0.498049458061175</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5022129561842534</v>
+        <v>0.5019505419388249</v>
       </c>
     </row>
     <row r="19">
@@ -1430,10 +1430,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5146610922144575</v>
+        <v>0.514760354218787</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4853389077855425</v>
+        <v>0.485239645781213</v>
       </c>
     </row>
     <row r="23">
@@ -1448,10 +1448,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5175939643420733</v>
+        <v>0.5153052426198728</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4824060356579268</v>
+        <v>0.4846947573801272</v>
       </c>
     </row>
     <row r="24">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.4470285044917383</v>
+        <v>0.4477647865174925</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5529714955082616</v>
+        <v>0.5522352134825075</v>
       </c>
     </row>
     <row r="29">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -1596,10 +1596,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.4351253691637335</v>
+        <v>0.4334053548128298</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5648746308362664</v>
+        <v>0.5665946451871702</v>
       </c>
     </row>
     <row r="34">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -1656,10 +1656,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.5044627784114113</v>
+        <v>0.5058599895644404</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4955372215885886</v>
+        <v>0.4941400104355596</v>
       </c>
     </row>
     <row r="38">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -1688,10 +1688,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.4205259815024008</v>
+        <v>0.4189023727609251</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5794740184975992</v>
+        <v>0.581097627239075</v>
       </c>
     </row>
     <row r="40">
@@ -1720,10 +1720,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.5593000638052517</v>
+        <v>0.5589542030282891</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4406999361947484</v>
+        <v>0.4410457969717108</v>
       </c>
     </row>
     <row r="42">
@@ -1738,10 +1738,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.488210146816955</v>
+        <v>0.4897837774194581</v>
       </c>
       <c r="D42" t="n">
-        <v>0.511789853183045</v>
+        <v>0.5102162225805418</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P.N.M.</t>
+          <t>U.N.C.</t>
         </is>
       </c>
     </row>
@@ -2176,10 +2176,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4889610636550767</v>
+        <v>0.4986999471354288</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5110389363449233</v>
+        <v>0.5013000528645712</v>
       </c>
     </row>
     <row r="3">
@@ -2194,10 +2194,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5180940068063941</v>
+        <v>0.5213918732611434</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4819059931936058</v>
+        <v>0.4786081267388564</v>
       </c>
     </row>
     <row r="4">
@@ -2212,10 +2212,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5637822502464083</v>
+        <v>0.5692839823501323</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4362177497535918</v>
+        <v>0.4307160176498677</v>
       </c>
     </row>
     <row r="5">
@@ -2230,10 +2230,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5282952703833925</v>
+        <v>0.5310794522270156</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4717047296166075</v>
+        <v>0.4689205477729845</v>
       </c>
     </row>
     <row r="6">
@@ -2248,10 +2248,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5426656043626547</v>
+        <v>0.5447250124667524</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4573343956373453</v>
+        <v>0.4552749875332476</v>
       </c>
     </row>
     <row r="7">
@@ -2266,10 +2266,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5451830479927785</v>
+        <v>0.537870978919868</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4548169520072216</v>
+        <v>0.4621290210801319</v>
       </c>
     </row>
     <row r="8">
@@ -2284,10 +2284,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.486202778353176</v>
+        <v>0.491102133507783</v>
       </c>
       <c r="D8" t="n">
-        <v>0.513797221646824</v>
+        <v>0.5088978664922169</v>
       </c>
     </row>
     <row r="9">
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4765708282371158</v>
+        <v>0.4718533505002138</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5234291717628842</v>
+        <v>0.5281466494997862</v>
       </c>
     </row>
     <row r="10">
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5339574664628861</v>
+        <v>0.5411531160569628</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4660425335371139</v>
+        <v>0.4588468839430372</v>
       </c>
     </row>
     <row r="11">
@@ -2338,10 +2338,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4648773638239581</v>
+        <v>0.4605997705688807</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5351226361760419</v>
+        <v>0.5394002294311193</v>
       </c>
     </row>
     <row r="12">
@@ -2356,10 +2356,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5816301228285838</v>
+        <v>0.5817175396086411</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4183698771714162</v>
+        <v>0.4182824603913588</v>
       </c>
     </row>
     <row r="13">
@@ -2374,10 +2374,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.520224448717577</v>
+        <v>0.5281978769981704</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4797755512824229</v>
+        <v>0.4718021230018296</v>
       </c>
     </row>
   </sheetData>
@@ -2433,10 +2433,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4504170482467472</v>
+        <v>0.4523889073091529</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5495829517532527</v>
+        <v>0.5476110926908471</v>
       </c>
     </row>
     <row r="3">
@@ -2451,10 +2451,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.485670021164641</v>
+        <v>0.4860478629936003</v>
       </c>
       <c r="D3" t="n">
-        <v>0.514329978835359</v>
+        <v>0.5139521370063997</v>
       </c>
     </row>
     <row r="4">
@@ -2469,10 +2469,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5390517578376165</v>
+        <v>0.5400631779254161</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4609482421623834</v>
+        <v>0.4599368220745839</v>
       </c>
     </row>
     <row r="5">
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4977870438157466</v>
+        <v>0.498049458061175</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5022129561842534</v>
+        <v>0.5019505419388249</v>
       </c>
     </row>
     <row r="6">
@@ -2505,10 +2505,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5146610922144575</v>
+        <v>0.514760354218787</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4853389077855425</v>
+        <v>0.485239645781213</v>
       </c>
     </row>
     <row r="7">
@@ -2523,10 +2523,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5175939643420733</v>
+        <v>0.5153052426198728</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4824060356579268</v>
+        <v>0.4846947573801272</v>
       </c>
     </row>
     <row r="8">
@@ -2541,10 +2541,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4470285044917383</v>
+        <v>0.4477647865174925</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5529714955082616</v>
+        <v>0.5522352134825075</v>
       </c>
     </row>
     <row r="9">
@@ -2559,10 +2559,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4351253691637335</v>
+        <v>0.4334053548128298</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5648746308362664</v>
+        <v>0.5665946451871702</v>
       </c>
     </row>
     <row r="10">
@@ -2577,10 +2577,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5044627784114113</v>
+        <v>0.5058599895644404</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4955372215885886</v>
+        <v>0.4941400104355596</v>
       </c>
     </row>
     <row r="11">
@@ -2595,10 +2595,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4205259815024008</v>
+        <v>0.4189023727609251</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5794740184975992</v>
+        <v>0.581097627239075</v>
       </c>
     </row>
     <row r="12">
@@ -2613,10 +2613,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5593000638052517</v>
+        <v>0.5589542030282891</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4406999361947484</v>
+        <v>0.4410457969717108</v>
       </c>
     </row>
     <row r="13">
@@ -2631,10 +2631,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.488210146816955</v>
+        <v>0.4897837774194581</v>
       </c>
       <c r="D13" t="n">
-        <v>0.511789853183045</v>
+        <v>0.5102162225805418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prediction margins added on hover
</commit_message>
<xml_diff>
--- a/2025_election_predictions.xlsx
+++ b/2025_election_predictions.xlsx
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.497331637795543</v>
+        <v>0.4973316377955416</v>
       </c>
       <c r="D4" t="n">
-        <v>0.502668362204457</v>
+        <v>0.5026683622044584</v>
       </c>
     </row>
     <row r="5">
@@ -545,10 +545,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5261620217177455</v>
+        <v>0.526162021717747</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4738379782822544</v>
+        <v>0.473837978282253</v>
       </c>
     </row>
     <row r="8">
@@ -605,10 +605,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5672478629219849</v>
+        <v>0.5672478629219884</v>
       </c>
       <c r="D11" t="n">
-        <v>0.432752137078015</v>
+        <v>0.4327521370780116</v>
       </c>
     </row>
     <row r="12">
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5426435505134022</v>
+        <v>0.5426435505134036</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4573564494865978</v>
+        <v>0.4573564494865964</v>
       </c>
     </row>
     <row r="19">
@@ -767,10 +767,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5460657010170746</v>
+        <v>0.5460657010170761</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4539342989829253</v>
+        <v>0.4539342989829239</v>
       </c>
     </row>
     <row r="23">
@@ -785,10 +785,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5415909534465717</v>
+        <v>0.5415909534465737</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4584090465534283</v>
+        <v>0.4584090465534262</v>
       </c>
     </row>
     <row r="24">
@@ -859,10 +859,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.504608837932104</v>
+        <v>0.5046088379321033</v>
       </c>
       <c r="D28" t="n">
-        <v>0.495391162067896</v>
+        <v>0.4953911620678967</v>
       </c>
     </row>
     <row r="29">
@@ -933,10 +933,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.4851247612759205</v>
+        <v>0.4851247612759185</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5148752387240795</v>
+        <v>0.5148752387240815</v>
       </c>
     </row>
     <row r="34">
@@ -993,10 +993,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.5450380227578381</v>
+        <v>0.5450380227578401</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4549619772421619</v>
+        <v>0.4549619772421599</v>
       </c>
     </row>
     <row r="38">
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.4631067436568784</v>
+        <v>0.4631067436568734</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5368932563431216</v>
+        <v>0.5368932563431266</v>
       </c>
     </row>
     <row r="40">
@@ -1057,10 +1057,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.5673490730438203</v>
+        <v>0.5673490730438236</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4326509269561797</v>
+        <v>0.4326509269561764</v>
       </c>
     </row>
     <row r="42">
@@ -1075,10 +1075,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.5278552419098032</v>
+        <v>0.527855241909804</v>
       </c>
       <c r="D42" t="n">
-        <v>0.4721447580901968</v>
+        <v>0.472144758090196</v>
       </c>
     </row>
   </sheetData>
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.45062702114528</v>
+        <v>0.4506270211452806</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5493729788547199</v>
+        <v>0.5493729788547195</v>
       </c>
     </row>
     <row r="5">
@@ -1208,10 +1208,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4919718609834932</v>
+        <v>0.4919718609834937</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5080281390165069</v>
+        <v>0.5080281390165061</v>
       </c>
     </row>
     <row r="8">
@@ -1268,10 +1268,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5376193076628931</v>
+        <v>0.5376193076628938</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4623806923371069</v>
+        <v>0.4623806923371063</v>
       </c>
     </row>
     <row r="12">
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5122258332396126</v>
+        <v>0.5122258332396132</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4877741667603875</v>
+        <v>0.4877741667603868</v>
       </c>
     </row>
     <row r="19">
@@ -1430,10 +1430,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5163901149031811</v>
+        <v>0.5163901149031818</v>
       </c>
       <c r="D22" t="n">
-        <v>0.483609885096819</v>
+        <v>0.4836098850968182</v>
       </c>
     </row>
     <row r="23">
@@ -1448,10 +1448,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5197647641313274</v>
+        <v>0.5197647641313282</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4802352358686726</v>
+        <v>0.480235235868672</v>
       </c>
     </row>
     <row r="24">
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.4649796771709884</v>
+        <v>0.4649796771709889</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5350203228290116</v>
+        <v>0.535020322829011</v>
       </c>
     </row>
     <row r="29">
@@ -1596,10 +1596,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.4503005998732688</v>
+        <v>0.4503005998732695</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5496994001267311</v>
+        <v>0.5496994001267305</v>
       </c>
     </row>
     <row r="34">
@@ -1656,10 +1656,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.5106404273295811</v>
+        <v>0.5106404273295817</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4893595726704189</v>
+        <v>0.4893595726704183</v>
       </c>
     </row>
     <row r="38">
@@ -1688,10 +1688,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.4221474005334988</v>
+        <v>0.4221474005334995</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5778525994665011</v>
+        <v>0.5778525994665006</v>
       </c>
     </row>
     <row r="40">
@@ -1720,10 +1720,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.5419776309578063</v>
+        <v>0.5419776309578069</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4580223690421937</v>
+        <v>0.4580223690421931</v>
       </c>
     </row>
     <row r="42">
@@ -1738,10 +1738,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.4893557649994206</v>
+        <v>0.4893557649994212</v>
       </c>
       <c r="D42" t="n">
-        <v>0.5106442350005793</v>
+        <v>0.5106442350005788</v>
       </c>
     </row>
   </sheetData>
@@ -2176,10 +2176,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.497331637795543</v>
+        <v>0.4973316377955416</v>
       </c>
       <c r="D2" t="n">
-        <v>0.502668362204457</v>
+        <v>0.5026683622044584</v>
       </c>
     </row>
     <row r="3">
@@ -2194,10 +2194,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5261620217177455</v>
+        <v>0.526162021717747</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4738379782822544</v>
+        <v>0.473837978282253</v>
       </c>
     </row>
     <row r="4">
@@ -2212,10 +2212,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5672478629219849</v>
+        <v>0.5672478629219884</v>
       </c>
       <c r="D4" t="n">
-        <v>0.432752137078015</v>
+        <v>0.4327521370780116</v>
       </c>
     </row>
     <row r="5">
@@ -2230,10 +2230,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5426435505134022</v>
+        <v>0.5426435505134036</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4573564494865978</v>
+        <v>0.4573564494865964</v>
       </c>
     </row>
     <row r="6">
@@ -2248,10 +2248,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5460657010170746</v>
+        <v>0.5460657010170761</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4539342989829253</v>
+        <v>0.4539342989829239</v>
       </c>
     </row>
     <row r="7">
@@ -2266,10 +2266,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5415909534465717</v>
+        <v>0.5415909534465737</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4584090465534283</v>
+        <v>0.4584090465534262</v>
       </c>
     </row>
     <row r="8">
@@ -2284,10 +2284,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.504608837932104</v>
+        <v>0.5046088379321033</v>
       </c>
       <c r="D8" t="n">
-        <v>0.495391162067896</v>
+        <v>0.4953911620678967</v>
       </c>
     </row>
     <row r="9">
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4851247612759205</v>
+        <v>0.4851247612759185</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5148752387240795</v>
+        <v>0.5148752387240815</v>
       </c>
     </row>
     <row r="10">
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5450380227578381</v>
+        <v>0.5450380227578401</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4549619772421619</v>
+        <v>0.4549619772421599</v>
       </c>
     </row>
     <row r="11">
@@ -2338,10 +2338,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4631067436568784</v>
+        <v>0.4631067436568734</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5368932563431216</v>
+        <v>0.5368932563431266</v>
       </c>
     </row>
     <row r="12">
@@ -2356,10 +2356,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5673490730438203</v>
+        <v>0.5673490730438236</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4326509269561797</v>
+        <v>0.4326509269561764</v>
       </c>
     </row>
     <row r="13">
@@ -2374,10 +2374,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.5278552419098032</v>
+        <v>0.527855241909804</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4721447580901968</v>
+        <v>0.472144758090196</v>
       </c>
     </row>
   </sheetData>
@@ -2433,10 +2433,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.45062702114528</v>
+        <v>0.4506270211452806</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5493729788547199</v>
+        <v>0.5493729788547195</v>
       </c>
     </row>
     <row r="3">
@@ -2451,10 +2451,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4919718609834932</v>
+        <v>0.4919718609834937</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5080281390165069</v>
+        <v>0.5080281390165061</v>
       </c>
     </row>
     <row r="4">
@@ -2469,10 +2469,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5376193076628931</v>
+        <v>0.5376193076628938</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4623806923371069</v>
+        <v>0.4623806923371063</v>
       </c>
     </row>
     <row r="5">
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5122258332396126</v>
+        <v>0.5122258332396132</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4877741667603875</v>
+        <v>0.4877741667603868</v>
       </c>
     </row>
     <row r="6">
@@ -2505,10 +2505,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5163901149031811</v>
+        <v>0.5163901149031818</v>
       </c>
       <c r="D6" t="n">
-        <v>0.483609885096819</v>
+        <v>0.4836098850968182</v>
       </c>
     </row>
     <row r="7">
@@ -2523,10 +2523,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5197647641313274</v>
+        <v>0.5197647641313282</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4802352358686726</v>
+        <v>0.480235235868672</v>
       </c>
     </row>
     <row r="8">
@@ -2541,10 +2541,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4649796771709884</v>
+        <v>0.4649796771709889</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5350203228290116</v>
+        <v>0.535020322829011</v>
       </c>
     </row>
     <row r="9">
@@ -2559,10 +2559,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4503005998732688</v>
+        <v>0.4503005998732695</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5496994001267311</v>
+        <v>0.5496994001267305</v>
       </c>
     </row>
     <row r="10">
@@ -2577,10 +2577,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5106404273295811</v>
+        <v>0.5106404273295817</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4893595726704189</v>
+        <v>0.4893595726704183</v>
       </c>
     </row>
     <row r="11">
@@ -2595,10 +2595,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4221474005334988</v>
+        <v>0.4221474005334995</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5778525994665011</v>
+        <v>0.5778525994665006</v>
       </c>
     </row>
     <row r="12">
@@ -2613,10 +2613,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5419776309578063</v>
+        <v>0.5419776309578069</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4580223690421937</v>
+        <v>0.4580223690421931</v>
       </c>
     </row>
     <row r="13">
@@ -2631,10 +2631,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.4893557649994206</v>
+        <v>0.4893557649994212</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5106442350005793</v>
+        <v>0.5106442350005788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>